<commit_message>
author pages working from clicking on tag
</commit_message>
<xml_diff>
--- a/CSV/poetry.xlsx
+++ b/CSV/poetry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/sampangk71280_masseyhigh_school_nz/Documents/COM301/Database/Poetry_DB/CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{743395A1-23B6-4C78-9508-9A1B11F3E4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB36BF7C-B72C-44B5-AFAB-844540A364AF}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{743395A1-23B6-4C78-9508-9A1B11F3E4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C5BFA0E-12EE-4BAA-99E5-45442542BAD7}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -16551,12 +16551,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I574"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView topLeftCell="A547" workbookViewId="0">
+      <selection activeCell="E576" sqref="E576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
@@ -33848,13 +33849,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13EB150B-2921-46CA-85FF-D8BFEE8BE2B1}">
   <dimension ref="A1:F574"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A534" workbookViewId="0">
+      <selection activeCell="C571" activeCellId="38" sqref="C14 C320 C331:C337 C342 C346 C349 C352 C359:C361 C375 C387 C393 C396 C406 C414 C416 C422 C431 C433 C435 C442 C445 C449 C460:C461 C469 C477 C480:C481 C492 C496 C507:C508 C515:C516 C518:C519 C523 C528 C531:C532 C534 C536:C537 C541:C543 C554 C571"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -45944,7 +45946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09021-4976-4603-85A6-6E7ED27F12CB}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>